<commit_message>
updated sound sources spreadsheet
</commit_message>
<xml_diff>
--- a/ChampionOfTheNine/Assets/Resources/Sounds/SoundSources.xlsx
+++ b/ChampionOfTheNine/Assets/Resources/Sounds/SoundSources.xlsx
@@ -377,7 +377,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,10 +414,6 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="str">
-        <f>C2&amp;" sound by "&amp;A2</f>
-        <v>Shotgun Blast sound by Jim Rogers</v>
-      </c>
     </row>
   </sheetData>
   <sortState ref="A2:C11">

</xml_diff>